<commit_message>
removed duplicate file and updated Rahil's tracker
</commit_message>
<xml_diff>
--- a/Assignments/Assignments Tracker.xlsx
+++ b/Assignments/Assignments Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\fs_ITMentoring_March2024\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08857C63-4C1E-44C5-82E9-14225726381B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD6A62-A82A-4DF4-B668-381B169EA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,6 @@
     <sheet name="Assignment Tracker" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xVZS5a/E8qws//PLhbk6vpqXulO7KwKAGCvX5FlAURA="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -190,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -227,6 +222,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -453,7 +451,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -542,12 +540,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="K2" s="15">
+        <v>1</v>
+      </c>
       <c r="L2" s="9">
         <v>1</v>
       </c>
@@ -578,12 +580,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="15">
+        <v>1</v>
+      </c>
       <c r="L3" s="9">
         <v>1</v>
       </c>
@@ -614,12 +620,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="K4" s="15">
+        <v>1</v>
+      </c>
       <c r="L4" s="9">
         <v>1</v>
       </c>
@@ -650,12 +660,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="K5" s="15">
+        <v>0.5</v>
+      </c>
       <c r="L5" s="9">
         <v>1</v>
       </c>
@@ -686,12 +700,16 @@
         <v>1</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
+      <c r="K6" s="15">
+        <v>1</v>
+      </c>
       <c r="L6" s="9">
         <v>1</v>
       </c>
@@ -722,12 +740,16 @@
         <v>1</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="K7" s="15">
+        <v>1</v>
+      </c>
       <c r="L7" s="9">
         <v>1</v>
       </c>
@@ -758,12 +780,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="K8" s="15">
+        <v>1</v>
+      </c>
       <c r="L8" s="9">
         <v>1</v>
       </c>
@@ -799,7 +825,9 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="K9" s="15">
+        <v>1</v>
+      </c>
       <c r="L9" s="9">
         <v>1</v>
       </c>
@@ -835,7 +863,9 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="15">
+        <v>1</v>
+      </c>
       <c r="L10" s="9">
         <v>1</v>
       </c>
@@ -871,7 +901,9 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="15">
+        <v>0.8</v>
+      </c>
       <c r="L11" s="9">
         <v>1</v>
       </c>

</xml_diff>